<commit_message>
cambios en Excel Especiales
</commit_message>
<xml_diff>
--- a/public/plantillas/plantillaespeciales.xlsx
+++ b/public/plantillas/plantillaespeciales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PlataformaComercial\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8E098D-6E14-45D6-BA33-FCDDFF3FCF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B954F718-6242-45C4-BB74-470FCAFB0280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{232DCA43-E593-4B73-8BFB-AD87ADD34780}"/>
   </bookViews>
@@ -35,33 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
-    <t>E01</t>
-  </si>
-  <si>
-    <t>E02</t>
-  </si>
-  <si>
-    <t>E03</t>
-  </si>
-  <si>
-    <t>E04</t>
-  </si>
-  <si>
-    <t>E05</t>
-  </si>
-  <si>
-    <t>E06</t>
-  </si>
-  <si>
-    <t>E07</t>
-  </si>
-  <si>
-    <t>E08</t>
-  </si>
-  <si>
-    <t>E09</t>
-  </si>
-  <si>
     <t>E10</t>
   </si>
   <si>
@@ -162,6 +135,33 @@
   </si>
   <si>
     <t>A6 NUEVOS ELECTRICOS</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
   </si>
 </sst>
 </file>
@@ -589,199 +589,199 @@
   <dimension ref="A1:U105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="T3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
cambios en Excel Especiales2.0
</commit_message>
<xml_diff>
--- a/public/plantillas/plantillaespeciales.xlsx
+++ b/public/plantillas/plantillaespeciales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PlataformaComercial\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B954F718-6242-45C4-BB74-470FCAFB0280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE74418-AEF7-426B-AFDA-AF71E7DBD3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{232DCA43-E593-4B73-8BFB-AD87ADD34780}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>E10</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>E9</t>
+  </si>
+  <si>
+    <t>E21</t>
+  </si>
+  <si>
+    <t>E22</t>
+  </si>
+  <si>
+    <t>Cierre</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -586,15 +598,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67B6D5A-5881-4F1F-85A1-02DD4B594B10}">
-  <dimension ref="A1:U105"/>
+  <dimension ref="A1:W105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -658,8 +670,14 @@
       <c r="U1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="6" t="s">
         <v>12</v>
@@ -721,8 +739,14 @@
       <c r="U2" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="V2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
@@ -783,8 +807,14 @@
       <c r="U3" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -806,7 +836,7 @@
       <c r="T4" s="9"/>
       <c r="U4" s="9"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -828,7 +858,7 @@
       <c r="T5" s="9"/>
       <c r="U5" s="9"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -850,7 +880,7 @@
       <c r="T6" s="9"/>
       <c r="U6" s="9"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -872,7 +902,7 @@
       <c r="T7" s="9"/>
       <c r="U7" s="9"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -894,7 +924,7 @@
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -916,7 +946,7 @@
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -938,7 +968,7 @@
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -960,7 +990,7 @@
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -982,7 +1012,7 @@
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1004,7 +1034,7 @@
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1026,7 +1056,7 @@
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1048,7 +1078,7 @@
       <c r="T15" s="5"/>
       <c r="U15" s="5"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>

</xml_diff>